<commit_message>
Update CAM_DVB-CI_v2.01_rev.2.01_BOM 2025-04-14 13-43.xlsx
</commit_message>
<xml_diff>
--- a/CAM_LATTICE_STM/ECAD/cam_dvb_ci_v2.01/Project Outputs for CAM_DVB-CI_v2.01/CAM_DVB-CI_v2.01_rev.2.01_BOM 2025-04-14 13-43.xlsx
+++ b/CAM_LATTICE_STM/ECAD/cam_dvb_ci_v2.01/Project Outputs for CAM_DVB-CI_v2.01/CAM_DVB-CI_v2.01_rev.2.01_BOM 2025-04-14 13-43.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Altium\SM_Project\CASS\CAM_LATTICE_STM\ECAD\cam_dvb_ci_v2.01\Project Outputs for CAM_DVB-CI_v2.01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIWA\Documents\GitHub\CASS\CAM_LATTICE_STM\ECAD\cam_dvb_ci_v2.01\Project Outputs for CAM_DVB-CI_v2.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27A72E77-D1CF-4349-A3AD-830E9FBE4016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FF8F50-EDCC-4AFF-96E8-6D0FFD201D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1482" yWindow="1542" windowWidth="17520" windowHeight="12138" xr2:uid="{A8CE955E-849A-4789-837B-063E29CA81ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A8CE955E-849A-4789-837B-063E29CA81ED}"/>
   </bookViews>
   <sheets>
     <sheet name="CAM_DVB-CI_v2.01_rev.2.01_BOM 2" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="149">
   <si>
     <t>Designator</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>HelpURL</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -216,12 +213,6 @@
     <t>IC11</t>
   </si>
   <si>
-    <t>LFE5U-25F-6BG256C</t>
-  </si>
-  <si>
-    <t>FPGA, 24K LUT, 137kbit RAM</t>
-  </si>
-  <si>
     <t>BGA256C80P16X16_1400X1400X170</t>
   </si>
   <si>
@@ -469,16 +460,62 @@
   </si>
   <si>
     <t>ASE-27.000MHZ-ET</t>
+  </si>
+  <si>
+    <t>Discontinued.</t>
+  </si>
+  <si>
+    <t>PCM-68P 卧贴</t>
+  </si>
+  <si>
+    <t>No need to install</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>REPLY</t>
+  </si>
+  <si>
+    <t>742C163330JP</t>
+  </si>
+  <si>
+    <t>LFE5U-45F-6BG256C</t>
+  </si>
+  <si>
+    <t>FPGA, 43.3K LUT, 137kbit RAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -523,18 +560,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{3AE70F0E-7F45-484F-B386-9DABBBDF7B67}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -846,20 +890,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3743AA8-A46B-4E00-A41B-D237CE9C4329}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="18.26171875" customWidth="1"/>
-    <col min="5" max="5" width="27.83984375" customWidth="1"/>
-    <col min="6" max="6" width="9.26171875" customWidth="1"/>
-    <col min="7" max="7" width="27.1015625" customWidth="1"/>
-    <col min="8" max="8" width="15.3125" customWidth="1"/>
+    <col min="1" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -881,823 +930,873 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="1">
         <v>33</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="F4" s="1">
         <v>5</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>5</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="1">
         <v>6</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="F8" s="1">
         <v>6</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F10" s="1">
         <v>6</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1">
         <v>4</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H18" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="F19" s="1">
         <v>3</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1">
         <v>7</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H21" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F23" s="1">
         <v>6</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2" t="s">
+      <c r="G24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2" t="s">
+      <c r="G25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="2" t="s">
+      <c r="G26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="F27" s="1">
         <v>9</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="2" t="s">
+      <c r="G27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="2" t="s">
+      <c r="G28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F29" s="1">
         <v>2</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="2" t="s">
+      <c r="G31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="F32" s="1">
         <v>6</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="2" t="s">
+      <c r="G32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="B33" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F35" s="1">
         <v>3</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="G36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>